<commit_message>
It has been a long time since any changes, huh?
</commit_message>
<xml_diff>
--- a/MS_MD101.xlsx
+++ b/MS_MD101.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c26969d82fe7094/Dokumenty/Personal/personalNotes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{9062759A-FED5-40A2-8783-59A483B5DA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B51A9908-C653-4494-B105-037A0A5429ED}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{9062759A-FED5-40A2-8783-59A483B5DA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45451E36-D666-4A57-B806-10A903C70DFA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C878DC24-42AC-4CA0-B89F-86E78E4EC3F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{C878DC24-42AC-4CA0-B89F-86E78E4EC3F6}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
+    <sheet name="Deployment" sheetId="2" r:id="rId2"/>
+    <sheet name="Identity, Compliance and Config" sheetId="3" r:id="rId3"/>
+    <sheet name="Maintain and Protect" sheetId="4" r:id="rId4"/>
+    <sheet name="Applications" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t xml:space="preserve"> - Používáním služby Windows Server Update Services mohou administrátoři plně spravovat distribuci aktualizací, uvolněných prostřednictvím Automatických aktualizací, do počítačů ve firemní síti</t>
   </si>
@@ -236,12 +240,192 @@
   <si>
     <t>Microsoft Endpoint Manager</t>
   </si>
+  <si>
+    <t>Deploy and upgrade operating systems</t>
+  </si>
+  <si>
+    <t>Assess infrastructure readiness</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Dodržováním osvědčených postupů a vyhýbáním se chybám při nasazení můžete zajistit, že vaši uživatelé budou produktivní a že projekt bude dodán podle plánu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Windows 10 je vydáván pomocí modelu nepřetržitého doručování známého jako Windows jako služba, přičemž nová verze Windows 10 je k dispozici každých šest měsíců</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Doporučuje se vybrat si skupinu uživatelů a nasadit Windows 10 do cílených pilotních projektů</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - To vám umožní otestovat každou verzi Windows 10 ve vaší organizaci před zavedením operačního systému pro větší kohorty uživatelů.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Rozdělením projektu nasazení Windows 10 do více fází můžete identifikovat jakékoli možné problémy a určit řešení, jsou-li k dispozici</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - To bude zahrnovat dokumentaci a získávání zpětné vazby od zúčastněných stran v každé fázi</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - První fáze nasazení operačního systému bude s </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pilotním nasazením</t>
+    </r>
+  </si>
+  <si>
+    <t>Pilot deployments</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Kontrolou a implementací zpětné vazby získané během pilotní fáze se můžete snažit minimalizovat budoucí dopad jakýchkoliv problémů, se kterými se setkáte</t>
+  </si>
+  <si>
+    <t>přehled o výhodách a potenciálních úskalích, se kterými se pravděpodobně setkáte v pozdějších fázíc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Pilotní projekt je nezbytný, protože může být užitečný pro zajištění kompatibility se stávajícím hardwarem, aplikacemi a infrastrukturou a poskytuje vám</t>
+  </si>
+  <si>
+    <t>V rámci pilotního projektu je důležité určit následující:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Produkční hardware, včetně počítačů, notebooků a tabletů, splňuje minimální hardwarové požadavky pro Windows 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Periferní zařízení, jako jsou tiskárny, skenery, projektory a další zařízení, jsou kompatibilní s Windows 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Všechny požadované ovladače zařízení jsou k dispozici</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Všechny aplikace požadované po nasazení budou fungovat ve Windows 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Jakékoli existující šifrování disku třetí strany bude fungovat s Windows 10 (alternativně nahrazeno šifrováním BitLocker Drive Encryption)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Vaši pracovníci IT podpory mají potřebné dovednosti pro podporu Windows 10</t>
+  </si>
+  <si>
+    <t>Verify hardware compatibility for multiple devices</t>
+  </si>
+  <si>
+    <t>MAP můžete použít k:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - Pokud máte tradiční on-premise infrastrukturu, můžete použít nástroj</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Microsoft Assessment and Planning Toolkit (MAP)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> k určení kompatibility/posouzení počítačových zařízení připojených k vaší síti</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Zjistit proveditelnost upgradu naskenovaných zařízení na Windows 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Zjistěte, zda je vaše organizace připravena přejít na Microsoft Azure, Office 365 nebo Azure AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Plán virtualizace pracovních zátěží na Hyper-V</t>
+  </si>
+  <si>
+    <t>Desktop Analytics</t>
+  </si>
+  <si>
+    <t>(To align investments with this shift, Desktop Analytics</t>
+  </si>
+  <si>
+    <t>will be retired on November 30, 2022. Over the next</t>
+  </si>
+  <si>
+    <t>year, the types of insights currently found in Desktop</t>
+  </si>
+  <si>
+    <t>Analytics will be incorporated directly into the Microsoft</t>
+  </si>
+  <si>
+    <t>Intune admin center.)</t>
+  </si>
+  <si>
+    <t>Evaluate and select an appropriate deployment option</t>
+  </si>
+  <si>
+    <t>Souhrnné srovnání mezi moderním dynamickým nasazování zařízení a tradičními metodami nasazení, které mohou zahrnovat i vytváření image</t>
+  </si>
+  <si>
+    <t>Dynamic provisioning methods</t>
+  </si>
+  <si>
+    <t>Traditional deployment methods</t>
+  </si>
+  <si>
+    <t>Device Management (Intune)</t>
+  </si>
+  <si>
+    <t>Enrollment into Azure Active Directory and Mobile</t>
+  </si>
+  <si>
+    <t>On-premises deployment tools using Windows ADK,</t>
+  </si>
+  <si>
+    <t>Windows Deployment Services, Microsoft Deployment</t>
+  </si>
+  <si>
+    <t>Toolkit, or Configuration Manager</t>
+  </si>
+  <si>
+    <t>Bare-metal install</t>
+  </si>
+  <si>
+    <t>Subscription Activation</t>
+  </si>
+  <si>
+    <t>In-place upgrade</t>
+  </si>
+  <si>
+    <t>Windows Autopilot</t>
+  </si>
+  <si>
+    <t>Wipe-and-load upgrade</t>
+  </si>
+  <si>
+    <t>Provisioning packages using Windows Configuration</t>
+  </si>
+  <si>
+    <t>Designer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,8 +479,41 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="5" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -339,8 +556,32 @@
         <bgColor rgb="FF666666"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -428,12 +669,131 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -446,33 +806,64 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,6 +941,18 @@
     <xdr:clientData/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -841,7 +1244,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -851,14 +1254,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{965EC74D-2DAE-4F4A-AF20-E2D94B45AB9C}">
   <dimension ref="A1:U66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B1" s="19"/>
@@ -867,7 +1270,7 @@
       <c r="E1" s="19"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
-      <c r="H1" s="18"/>
+      <c r="H1" s="20"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -883,14 +1286,14 @@
       <c r="U1" s="1"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="15"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
       <c r="I2" s="2" t="s">
         <v>35</v>
       </c>
@@ -908,14 +1311,14 @@
       <c r="U2" s="1"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="15"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -931,14 +1334,14 @@
       <c r="U3" s="1"/>
     </row>
     <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="12"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="26"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -2456,4 +2859,365 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB3BBE4-855A-4862-A62F-3BA2FBAF7A86}">
+  <dimension ref="A2:H55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C37" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C38" s="28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C39" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C40" s="28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="15"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F47" s="34"/>
+      <c r="G47" s="34"/>
+      <c r="H47" s="35"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" s="30"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="37"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" s="30"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="F49" s="30"/>
+      <c r="G49" s="30"/>
+      <c r="H49" s="37"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="36"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="F50" s="30"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="37"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F51" s="30"/>
+      <c r="G51" s="30"/>
+      <c r="H51" s="37"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" s="30"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="30"/>
+      <c r="G52" s="30"/>
+      <c r="H52" s="37"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53" s="30"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="F53" s="30"/>
+      <c r="G53" s="30"/>
+      <c r="H53" s="37"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" s="30"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F54" s="30"/>
+      <c r="G54" s="30"/>
+      <c r="H54" s="37"/>
+    </row>
+    <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="38"/>
+      <c r="B55" s="39"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="E47:H47"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D281211-7DDD-48AE-8DE6-3DAE8F28335F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12FDD799-7B99-4496-988E-84F118F477F5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55274CB1-A09A-4F28-AE7E-101018467B60}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>